<commit_message>
updated with a few small fixes
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SheetA" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Monkey" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SheetA" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="14">
   <si>
     <t xml:space="preserve">Who am I</t>
   </si>
@@ -76,6 +77,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -159,13 +161,13 @@
   </sheetPr>
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20:A25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,4 +1257,1109 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D77"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
do not fail on the odd missing fields
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Monkey" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="This be a sheet" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SheetA" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -161,14 +161,11 @@
   </sheetPr>
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1266,14 +1263,11 @@
   </sheetPr>
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2356,7 +2350,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>